<commit_message>
made changes to excel data
</commit_message>
<xml_diff>
--- a/SGA_Example_DataSet.xlsx
+++ b/SGA_Example_DataSet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kopot\Desktop\Work\SGA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kopot\Documents\SGA-Tutorial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07A01306-C5BA-4CD9-B845-87839C0145EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E02F3C1-0D5F-43A3-9B76-24EDBD176A5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -80,7 +80,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="174" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -114,7 +114,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -398,7 +398,7 @@
   <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="K7" sqref="K7:M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -452,37 +452,37 @@
         <v>0.28895631014718814</v>
       </c>
       <c r="C2" s="2">
-        <v>0.12478348523298807</v>
+        <v>6.5425817545498074E-2</v>
       </c>
       <c r="D2" s="2">
-        <v>0.57130065785162376</v>
+        <v>8.3402857461769106E-2</v>
       </c>
       <c r="E2" s="2">
-        <v>1.3068142786444452</v>
+        <v>8.5074607013506665E-2</v>
       </c>
       <c r="F2" s="2">
         <v>0.21786346603467102</v>
       </c>
       <c r="G2" s="2">
-        <v>1.0303478876728607</v>
+        <v>0.50530815326913325</v>
       </c>
       <c r="H2" s="2">
-        <v>0.68385577879335258</v>
+        <v>0.5354995420627251</v>
       </c>
       <c r="I2" s="2">
-        <v>1.1142533705481352</v>
+        <v>0.46682690012958195</v>
       </c>
       <c r="J2" s="2">
         <v>0.37667372287496964</v>
       </c>
       <c r="K2" s="2">
-        <v>1.1683081240720516</v>
+        <v>0.6839633541202238</v>
       </c>
       <c r="L2" s="2">
-        <v>0.25024548215337372</v>
+        <v>0.68887933498988096</v>
       </c>
       <c r="M2" s="2">
-        <v>0.62226312337525447</v>
+        <v>0.68017530472697529</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
@@ -493,37 +493,37 @@
         <v>0.3355625764999865</v>
       </c>
       <c r="C3" s="2">
-        <v>0.53404184100845087</v>
+        <v>0.21795111073291168</v>
       </c>
       <c r="D3" s="2">
-        <v>0.20936964884460726</v>
+        <v>0.26577160041705661</v>
       </c>
       <c r="E3" s="2">
-        <v>1.0601220816468018</v>
+        <v>0.26049996470420211</v>
       </c>
       <c r="F3" s="2">
         <v>0.26355242865601991</v>
       </c>
       <c r="G3" s="2">
-        <v>1.5919978876476775</v>
+        <v>0.66667698199173264</v>
       </c>
       <c r="H3" s="2">
-        <v>9.6722858658106758E-2</v>
+        <v>0.66104406028723295</v>
       </c>
       <c r="I3" s="2">
-        <v>1.3613065447450174</v>
+        <v>0.67208950937490675</v>
       </c>
       <c r="J3" s="2">
         <v>0.2255144421569889</v>
       </c>
       <c r="K3" s="2">
-        <v>0.31960857615575106</v>
+        <v>0.6165022570187868</v>
       </c>
       <c r="L3" s="2">
-        <v>1.0838418930687201</v>
+        <v>0.71095215165482384</v>
       </c>
       <c r="M3" s="2">
-        <v>0.71256259769565489</v>
+        <v>0.71474657617833626</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
@@ -534,37 +534,37 @@
         <v>0.31571102798021544</v>
       </c>
       <c r="C4" s="2">
-        <v>0.71413474056257864</v>
+        <v>0.58468356609556871</v>
       </c>
       <c r="D4" s="2">
-        <v>1.5322782833570403</v>
+        <v>0.40250378461243119</v>
       </c>
       <c r="E4" s="2">
-        <v>1.4264121157116008</v>
+        <v>0.43174604912019598</v>
       </c>
       <c r="F4" s="2">
         <v>0.35103767094807459</v>
       </c>
       <c r="G4" s="2">
-        <v>1.0196419861115047</v>
+        <v>0.78416489251241528</v>
       </c>
       <c r="H4" s="2">
-        <v>1.1241588745790851</v>
+        <v>0.80785471333946324</v>
       </c>
       <c r="I4" s="2">
-        <v>0.37924037666593818</v>
+        <v>0.83870556540950769</v>
       </c>
       <c r="J4" s="2">
         <v>0.39221484283797403</v>
       </c>
       <c r="K4" s="2">
-        <v>1.3199487830705421</v>
+        <v>1.1382623304165369</v>
       </c>
       <c r="L4" s="2">
-        <v>1.5318979827688275</v>
+        <v>1.2667277509561061</v>
       </c>
       <c r="M4" s="2">
-        <v>1.0807657706746507</v>
+        <v>1.0254000356315971</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
@@ -575,37 +575,37 @@
         <v>0.32439399763784371</v>
       </c>
       <c r="C5" s="2">
-        <v>0.88817320315068993</v>
+        <v>0.86282502387673077</v>
       </c>
       <c r="D5" s="2">
-        <v>0.1716575144389029</v>
+        <v>0.77762469642360887</v>
       </c>
       <c r="E5" s="2">
-        <v>1.3203620376571883</v>
+        <v>0.83284727546183213</v>
       </c>
       <c r="F5" s="2">
         <v>0.21449590089764684</v>
       </c>
       <c r="G5" s="2">
-        <v>0.78967671491160352</v>
+        <v>0.48335264027604857</v>
       </c>
       <c r="H5" s="2">
-        <v>1.3942151066277788</v>
+        <v>0.78493709588235883</v>
       </c>
       <c r="I5" s="2">
-        <v>1.3316990433988372</v>
+        <v>0.85109763632603164</v>
       </c>
       <c r="J5" s="2">
         <v>0.20382660907313674</v>
       </c>
       <c r="K5" s="2">
-        <v>1.4824044047295153</v>
+        <v>1.28498605292826</v>
       </c>
       <c r="L5" s="2">
-        <v>0.11999670552548791</v>
+        <v>1.2258668584710559</v>
       </c>
       <c r="M5" s="2">
-        <v>0.39818931987333528</v>
+        <v>1.2347671776924947</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">

</xml_diff>